<commit_message>
added well log content model
added well log content model
</commit_message>
<xml_diff>
--- a/Classes/Attribute.xlsx
+++ b/Classes/Attribute.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\MIXITE\Projects\Geothermal_DOE\ContentModelsDevelopment\Linked Data Registry\Classes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Geothermal_DOE\ContentModelsDevelopment\Linked Data Registry\Classes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -6295,37 +6295,7 @@
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -6658,7 +6628,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomRight" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8777,40 +8747,37 @@
         <v>359</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B106,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/depth-ft</v>
+        <v>class/attribute/depthbottominterval</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1898</v>
+        <v>1869</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>1366</v>
       </c>
-      <c r="G106" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="107" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B107,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/depthbottominterval</v>
+        <v>class/attribute/depthbottominterval-ft</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>1869</v>
+        <v>1896</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>1366</v>
@@ -8819,55 +8786,58 @@
     <row r="108" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B108,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/depthbottominterval-ft</v>
+        <v>class/attribute/depthbottomopenzone</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>1896</v>
+        <v>1870</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>1366</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B109,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/depthbottomopenzone</v>
+        <v>class/attribute/depthdeterminationmethod</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>1870</v>
+        <v>1676</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>1366</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" ht="99.75" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B110,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/depthdeterminationmethod</v>
+        <v>class/attribute/depth-ft</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1676</v>
+        <v>1898</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>4</v>
+        <v>1366</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
@@ -9574,115 +9544,115 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="57" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B148,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/elevation-ft-msl</v>
+        <v>class/attribute/elevationbottomopenzone-msl</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>1878</v>
+        <v>1880</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="F148" s="1" t="s">
         <v>1366</v>
       </c>
-      <c r="H148" s="1" t="s">
-        <v>1980</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" ht="57" x14ac:dyDescent="0.2">
+    </row>
+    <row r="149" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B149,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/elevation-m</v>
+        <v>class/attribute/elevationdatum</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>1879</v>
+        <v>1856</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>446</v>
+        <v>353</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>1366</v>
-      </c>
-      <c r="H149" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="150" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B150,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/elevationbottomopenzone-msl</v>
+        <v>class/attribute/elevationdatum-m</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>1880</v>
+        <v>1858</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>448</v>
+        <v>353</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>1366</v>
       </c>
     </row>
-    <row r="151" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B151,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/elevationdatum</v>
+        <v>class/attribute/elevationdf</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>1856</v>
+        <v>1441</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>353</v>
+        <v>452</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+        <v>1366</v>
+      </c>
+      <c r="G151" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B152,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/elevationdatum-m</v>
+        <v>class/attribute/elevation-ft-msl</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>1858</v>
+        <v>1878</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>353</v>
+        <v>444</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>1366</v>
+      </c>
+      <c r="H152" s="1" t="s">
+        <v>1980</v>
       </c>
     </row>
     <row r="153" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B153,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/elevationdf</v>
+        <v>class/attribute/elevationgl</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="F153" s="1" t="s">
         <v>1366</v>
@@ -9694,16 +9664,16 @@
     <row r="154" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B154,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/elevationgl</v>
+        <v>class/attribute/elevationgl-ft</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>1442</v>
+        <v>1792</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="F154" s="1" t="s">
         <v>1366</v>
@@ -9711,44 +9681,44 @@
       <c r="G154" s="1" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="H154" s="1" t="s">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B155,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/elevationgl-ft</v>
+        <v>class/attribute/elevationgl-m</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="F155" s="1" t="s">
         <v>1366</v>
       </c>
       <c r="G155" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="H155" s="1" t="s">
-        <v>1980</v>
       </c>
     </row>
     <row r="156" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B156,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/elevationgl-m</v>
+        <v>class/attribute/elevationkb</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>1791</v>
+        <v>1443</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="F156" s="1" t="s">
         <v>1366</v>
@@ -9760,22 +9730,22 @@
     <row r="157" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B157,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/elevationkb</v>
+        <v>class/attribute/elevation-m</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>459</v>
+        <v>445</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>1443</v>
+        <v>1879</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>460</v>
+        <v>446</v>
       </c>
       <c r="F157" s="1" t="s">
         <v>1366</v>
       </c>
-      <c r="G157" s="1" t="s">
-        <v>417</v>
+      <c r="H157" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="158" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
@@ -10006,19 +9976,19 @@
         <v>191</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B170,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/eqlog-totaldepth</v>
+        <v>class/attribute/eqlogtemperaturebottom</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>1860</v>
+        <v>1803</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="F170" s="1" t="s">
         <v>1366</v>
@@ -10027,16 +9997,16 @@
     <row r="171" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B171,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/eqlogtemperaturebottom</v>
+        <v>class/attribute/eqlogtemperaturemax</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>1803</v>
+        <v>1804</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="F171" s="1" t="s">
         <v>1366</v>
@@ -10045,16 +10015,16 @@
     <row r="172" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B172,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/eqlogtemperaturemax</v>
+        <v>class/attribute/eqlogtemperaturetop</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>1804</v>
+        <v>1805</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="F172" s="1" t="s">
         <v>1366</v>
@@ -10063,16 +10033,16 @@
     <row r="173" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B173,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/eqlogtemperaturetop</v>
+        <v>class/attribute/eqlog-totaldepth</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>1805</v>
+        <v>1860</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>1366</v>
@@ -10832,49 +10802,49 @@
       <c r="H212" s="6"/>
       <c r="I212" s="6"/>
     </row>
-    <row r="213" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:9" ht="57" x14ac:dyDescent="0.2">
       <c r="A213" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B213,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/fluidtemperature-c</v>
+        <v>class/attribute/fluidtemperaturec</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>545</v>
+        <v>1483</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>1808</v>
+        <v>101</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>546</v>
+        <v>100</v>
       </c>
       <c r="F213" s="1" t="s">
         <v>1366</v>
       </c>
       <c r="G213" s="1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="214" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="H213" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A214" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B214,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/fluidtemperaturec</v>
+        <v>class/attribute/fluidtemperature-c</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>1483</v>
+        <v>545</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>101</v>
+        <v>1808</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>100</v>
+        <v>546</v>
       </c>
       <c r="F214" s="1" t="s">
         <v>1366</v>
       </c>
       <c r="G214" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="H214" s="1" t="s">
-        <v>98</v>
+        <v>417</v>
       </c>
     </row>
     <row r="215" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
@@ -11339,19 +11309,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="239" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A239" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B239,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/grossproduction-mwhr</v>
-      </c>
-      <c r="B239" s="2" t="s">
-        <v>2034</v>
-      </c>
-      <c r="C239" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D239" s="2" t="s">
-        <v>147</v>
+        <v>class/attribute/grossproductioncapacity</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>1389</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>591</v>
       </c>
       <c r="F239" s="1" t="s">
         <v>1366</v>
@@ -11360,16 +11330,16 @@
     <row r="240" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A240" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B240,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/grossproductioncapacity</v>
-      </c>
-      <c r="B240" s="1" t="s">
-        <v>590</v>
-      </c>
-      <c r="C240" s="1" t="s">
-        <v>1389</v>
-      </c>
-      <c r="D240" s="1" t="s">
-        <v>591</v>
+        <v>class/attribute/grossproduction-mwhr</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>2034</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D240" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="F240" s="1" t="s">
         <v>1366</v>
@@ -12775,7 +12745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="315" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A315" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B315,",",""),"_","-")," ","-"))</f>
         <v>class/attribute/localityterms</v>
@@ -12811,7 +12781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="317" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A317" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B317,",",""),"_","-")," ","-"))</f>
         <v>class/attribute/locationkeyword</v>
@@ -12829,7 +12799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="318" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A318" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B318,",",""),"_","-")," ","-"))</f>
         <v>class/attribute/locationname</v>
@@ -13706,13 +13676,13 @@
     <row r="363" spans="1:7" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A363" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B363,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/metadata-uri</v>
+        <v>class/attribute/metadatauri</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>797</v>
+        <v>63</v>
       </c>
       <c r="C363" s="1" t="s">
-        <v>1774</v>
+        <v>63</v>
       </c>
       <c r="D363" s="1" t="s">
         <v>62</v>
@@ -13727,13 +13697,13 @@
     <row r="364" spans="1:7" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A364" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B364,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/metadatauri</v>
+        <v>class/attribute/metadata-uri</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>63</v>
+        <v>797</v>
       </c>
       <c r="C364" s="1" t="s">
-        <v>63</v>
+        <v>1774</v>
       </c>
       <c r="D364" s="1" t="s">
         <v>62</v>
@@ -13745,7 +13715,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="365" spans="1:7" ht="142.5" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:7" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A365" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B365,",",""),"_","-")," ","-"))</f>
         <v>class/attribute/methodology</v>
@@ -13817,7 +13787,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="369" spans="1:7" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:7" ht="57" x14ac:dyDescent="0.2">
       <c r="A369" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B369,",",""),"_","-")," ","-"))</f>
         <v>class/attribute/mineoropeningtype</v>
@@ -13895,7 +13865,7 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="373" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A373" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B373,",",""),"_","-")," ","-"))</f>
         <v>class/attribute/minhf-kjyr</v>
@@ -14615,7 +14585,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="411" spans="1:7" ht="128.25" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:7" ht="114" x14ac:dyDescent="0.2">
       <c r="A411" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B411,",",""),"_","-")," ","-"))</f>
         <v>class/attribute/origindatetime</v>
@@ -14789,7 +14759,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="420" spans="1:7" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:7" ht="57" x14ac:dyDescent="0.2">
       <c r="A420" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B420,",",""),"_","-")," ","-"))</f>
         <v>class/attribute/otherlocationinformation</v>
@@ -14807,7 +14777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="421" spans="1:7" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:7" ht="57" x14ac:dyDescent="0.2">
       <c r="A421" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B421,",",""),"_","-")," ","-"))</f>
         <v>class/attribute/otherlocationname</v>
@@ -14849,7 +14819,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="423" spans="1:7" ht="156.75" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:7" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A423" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B423,",",""),"_","-")," ","-"))</f>
         <v>class/attribute/othername</v>
@@ -15110,200 +15080,200 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="436" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A436" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B436,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/permeability-md</v>
+        <v>class/attribute/permeabilityair-md</v>
       </c>
       <c r="B436" s="2" t="s">
-        <v>1737</v>
+        <v>2037</v>
       </c>
       <c r="C436" s="2" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D436" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="437" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="437" spans="1:8" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A437" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B437,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/permeabilityair-md</v>
-      </c>
-      <c r="B437" s="2" t="s">
-        <v>2037</v>
-      </c>
-      <c r="C437" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D437" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="438" spans="1:8" ht="85.5" x14ac:dyDescent="0.2">
+        <v>class/attribute/permeabilityaverage-m2</v>
+      </c>
+      <c r="B437" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="C437" s="1" t="s">
+        <v>1929</v>
+      </c>
+      <c r="D437" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="F437" s="1" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="438" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A438" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B438,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/permeabilityaverage-m2</v>
+        <v>class/attribute/permeabilityaveragemethod</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="C438" s="1" t="s">
-        <v>1929</v>
+        <v>1686</v>
       </c>
       <c r="D438" s="1" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="F438" s="1" t="s">
-        <v>1366</v>
+        <v>4</v>
       </c>
     </row>
     <row r="439" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A439" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B439,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/permeabilityaveragemethod</v>
+        <v>class/attribute/permeabilityaverageuncertainty</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="C439" s="1" t="s">
-        <v>1686</v>
+        <v>1836</v>
       </c>
       <c r="D439" s="1" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="F439" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="440" spans="1:8" ht="57" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A440" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B440,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/permeabilityaverageuncertainty</v>
-      </c>
-      <c r="B440" s="1" t="s">
-        <v>912</v>
-      </c>
-      <c r="C440" s="1" t="s">
-        <v>1836</v>
-      </c>
-      <c r="D440" s="1" t="s">
-        <v>913</v>
-      </c>
-      <c r="F440" s="1" t="s">
-        <v>4</v>
+        <v>class/attribute/permeabilitycommonlyobserved-md</v>
+      </c>
+      <c r="B440" s="2" t="s">
+        <v>1738</v>
+      </c>
+      <c r="C440" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D440" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="441" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A441" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B441,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/permeabilitycommonlyobserved-md</v>
+        <v>class/attribute/permeabilitygeometricmean-md</v>
       </c>
       <c r="B441" s="2" t="s">
-        <v>1738</v>
+        <v>1739</v>
       </c>
       <c r="C441" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D441" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="442" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+      <c r="H441" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="442" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A442" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B442,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/permeabilitygeometricmean-md</v>
+        <v>class/attribute/permeabilityintrinsic-md</v>
       </c>
       <c r="B442" s="2" t="s">
-        <v>1739</v>
+        <v>1734</v>
       </c>
       <c r="C442" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D442" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="H442" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="443" spans="1:8" ht="57" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A443" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B443,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/permeabilityintrinsic-md</v>
+        <v>class/attribute/permeabilitylocal-md</v>
       </c>
       <c r="B443" s="2" t="s">
-        <v>1734</v>
+        <v>1732</v>
       </c>
       <c r="C443" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D443" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H443" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="444" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+      <c r="D443" s="2"/>
+    </row>
+    <row r="444" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A444" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B444,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/permeabilitylocal-md</v>
-      </c>
-      <c r="B444" s="2" t="s">
-        <v>1732</v>
-      </c>
-      <c r="C444" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D444" s="2"/>
-    </row>
-    <row r="445" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+        <v>class/attribute/permeabilitymax-m2</v>
+      </c>
+      <c r="B444" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="C444" s="1" t="s">
+        <v>1930</v>
+      </c>
+      <c r="D444" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="F444" s="1" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="445" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A445" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B445,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/permeabilitymax-m2</v>
-      </c>
-      <c r="B445" s="1" t="s">
-        <v>914</v>
-      </c>
-      <c r="C445" s="1" t="s">
-        <v>1930</v>
-      </c>
-      <c r="D445" s="1" t="s">
-        <v>915</v>
-      </c>
-      <c r="F445" s="1" t="s">
-        <v>1366</v>
-      </c>
-    </row>
-    <row r="446" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
+        <v>class/attribute/permeability-md</v>
+      </c>
+      <c r="B445" s="2" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C445" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D445" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="446" spans="1:8" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A446" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B446,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/permeabilitymean-md</v>
+        <v>class/attribute/permeabilitymeanintrinsic-md</v>
       </c>
       <c r="B446" s="2" t="s">
-        <v>1740</v>
+        <v>1733</v>
       </c>
       <c r="C446" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D446" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="447" spans="1:8" ht="85.5" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="447" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A447" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B447,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/permeabilitymeanintrinsic-md</v>
+        <v>class/attribute/permeabilitymean-md</v>
       </c>
       <c r="B447" s="2" t="s">
-        <v>1733</v>
+        <v>1740</v>
       </c>
       <c r="C447" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D447" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="448" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
@@ -15554,40 +15524,40 @@
         <v>4</v>
       </c>
     </row>
-    <row r="462" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:7" ht="57" x14ac:dyDescent="0.2">
       <c r="A462" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B462,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/plss-meridians</v>
+        <v>class/attribute/plsslocation</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>45</v>
+        <v>1998</v>
       </c>
       <c r="C462" s="1" t="s">
-        <v>1934</v>
+        <v>1999</v>
       </c>
       <c r="D462" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E462" s="1" t="s">
-        <v>17</v>
+        <v>2000</v>
       </c>
       <c r="F462" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="463" spans="1:7" ht="57" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A463" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B463,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/plsslocation</v>
+        <v>class/attribute/plss-meridians</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>1998</v>
+        <v>45</v>
       </c>
       <c r="C463" s="1" t="s">
-        <v>1999</v>
+        <v>1934</v>
       </c>
       <c r="D463" s="1" t="s">
-        <v>2000</v>
+        <v>44</v>
+      </c>
+      <c r="E463" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="F463" s="1" t="s">
         <v>4</v>
@@ -15686,40 +15656,40 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="468" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A468" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B468,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/porosityaverage-pct</v>
+        <v>class/attribute/porosityaveragemethod</v>
       </c>
       <c r="B468" s="1" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="C468" s="1" t="s">
-        <v>1935</v>
+        <v>1687</v>
       </c>
       <c r="D468" s="1" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="F468" s="1" t="s">
-        <v>1366</v>
-      </c>
-    </row>
-    <row r="469" spans="1:8" ht="57" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="469" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A469" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B469,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/porosityaveragemethod</v>
+        <v>class/attribute/porosityaverage-pct</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="C469" s="1" t="s">
-        <v>1687</v>
+        <v>1935</v>
       </c>
       <c r="D469" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="F469" s="1" t="s">
-        <v>4</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="470" spans="1:8" ht="57" x14ac:dyDescent="0.2">
@@ -15955,55 +15925,55 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="483" spans="1:7" ht="57" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A483" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B483,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/pressure-psi</v>
+        <v>class/attribute/pressurefinalshutin</v>
       </c>
       <c r="B483" s="1" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="C483" s="1" t="s">
-        <v>1938</v>
+        <v>1712</v>
       </c>
       <c r="D483" s="1" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="F483" s="1" t="s">
         <v>1366</v>
       </c>
     </row>
-    <row r="484" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A484" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B484,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/pressurefinalshutin</v>
+        <v>class/attribute/pressureinitialshutin</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="C484" s="1" t="s">
-        <v>1712</v>
+        <v>1710</v>
       </c>
       <c r="D484" s="1" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="F484" s="1" t="s">
         <v>1366</v>
       </c>
     </row>
-    <row r="485" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:7" ht="57" x14ac:dyDescent="0.2">
       <c r="A485" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B485,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/pressureinitialshutin</v>
+        <v>class/attribute/pressure-psi</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>953</v>
+        <v>949</v>
       </c>
       <c r="C485" s="1" t="s">
-        <v>1710</v>
+        <v>1938</v>
       </c>
       <c r="D485" s="1" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
       <c r="F485" s="1" t="s">
         <v>1366</v>
@@ -16851,7 +16821,7 @@
       <c r="H529" s="1"/>
       <c r="I529" s="1"/>
     </row>
-    <row r="530" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="530" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A530" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B530,",",""),"_","-")," ","-"))</f>
         <v>class/attribute/samplecollectionmethod</v>
@@ -17038,7 +17008,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="540" spans="1:9" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="540" spans="1:9" ht="57" x14ac:dyDescent="0.2">
       <c r="A540" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B540,",",""),"_","-")," ","-"))</f>
         <v>class/attribute/sampledgeologicunit</v>
@@ -17431,94 +17401,94 @@
     <row r="561" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A561" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B561,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/se-uncorrectedgradient</v>
+        <v>class/attribute/section-</v>
       </c>
       <c r="B561" s="1" t="s">
-        <v>1082</v>
+        <v>1086</v>
       </c>
       <c r="C561" s="1" t="s">
-        <v>1843</v>
+        <v>1941</v>
       </c>
       <c r="D561" s="1" t="s">
-        <v>1083</v>
+        <v>35</v>
       </c>
       <c r="F561" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="562" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="G561" s="1" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="562" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A562" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B562,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/se-uncorrectedheatflow</v>
+        <v>class/attribute/sectionpart</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1084</v>
+        <v>1087</v>
       </c>
       <c r="C562" s="1" t="s">
-        <v>1844</v>
+        <v>1612</v>
       </c>
       <c r="D562" s="1" t="s">
-        <v>1085</v>
+        <v>32</v>
       </c>
       <c r="F562" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="563" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="G562" s="1" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="563" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A563" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B563,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/section-</v>
+        <v>class/attribute/seisometernetwork</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>1086</v>
+        <v>1088</v>
       </c>
       <c r="C563" s="1" t="s">
-        <v>1941</v>
+        <v>1578</v>
       </c>
       <c r="D563" s="1" t="s">
-        <v>35</v>
+        <v>1089</v>
       </c>
       <c r="F563" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G563" s="1" t="s">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="564" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="564" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A564" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B564,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/sectionpart</v>
+        <v>class/attribute/se-uncorrectedgradient</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>1087</v>
+        <v>1082</v>
       </c>
       <c r="C564" s="1" t="s">
-        <v>1612</v>
+        <v>1843</v>
       </c>
       <c r="D564" s="1" t="s">
-        <v>32</v>
+        <v>1083</v>
       </c>
       <c r="F564" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G564" s="1" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="565" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="565" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A565" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B565,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/seisometernetwork</v>
+        <v>class/attribute/se-uncorrectedheatflow</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1088</v>
+        <v>1084</v>
       </c>
       <c r="C565" s="1" t="s">
-        <v>1578</v>
+        <v>1844</v>
       </c>
       <c r="D565" s="1" t="s">
-        <v>1089</v>
+        <v>1085</v>
       </c>
       <c r="F565" s="1" t="s">
         <v>4</v>
@@ -17575,7 +17545,7 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="569" spans="1:7" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="569" spans="1:7" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A569" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B569,",",""),"_","-")," ","-"))</f>
         <v>class/attribute/shutinpressuremethod</v>
@@ -17830,19 +17800,19 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="582" spans="1:7" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="582" spans="1:7" ht="114" x14ac:dyDescent="0.2">
       <c r="A582" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B582,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/specification-uri</v>
+        <v>class/attribute/specificationuri</v>
       </c>
       <c r="B582" s="1" t="s">
-        <v>1113</v>
+        <v>1114</v>
       </c>
       <c r="C582" s="1" t="s">
-        <v>1945</v>
+        <v>1505</v>
       </c>
       <c r="D582" s="1" t="s">
-        <v>108</v>
+        <v>1115</v>
       </c>
       <c r="F582" s="1" t="s">
         <v>61</v>
@@ -17851,19 +17821,19 @@
         <v>60</v>
       </c>
     </row>
-    <row r="583" spans="1:7" ht="114" x14ac:dyDescent="0.2">
+    <row r="583" spans="1:7" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A583" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B583,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/specificationuri</v>
+        <v>class/attribute/specification-uri</v>
       </c>
       <c r="B583" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="C583" s="1" t="s">
-        <v>1505</v>
+        <v>1945</v>
       </c>
       <c r="D583" s="1" t="s">
-        <v>1115</v>
+        <v>108</v>
       </c>
       <c r="F583" s="1" t="s">
         <v>61</v>
@@ -17944,7 +17914,7 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="588" spans="1:7" ht="114" x14ac:dyDescent="0.2">
+    <row r="588" spans="1:7" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A588" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B588,",",""),"_","-")," ","-"))</f>
         <v>class/attribute/specificyield-percent</v>
@@ -18373,7 +18343,7 @@
         <v>1978</v>
       </c>
     </row>
-    <row r="610" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="610" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A610" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B610,",",""),"_","-")," ","-"))</f>
         <v>class/attribute/status</v>
@@ -18598,37 +18568,37 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="622" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="622" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A622" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B622,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/temperature-f</v>
+        <v>class/attribute/temperaturecorrection</v>
       </c>
       <c r="B622" s="1" t="s">
-        <v>1175</v>
+        <v>1177</v>
       </c>
       <c r="C622" s="1" t="s">
-        <v>1816</v>
+        <v>1463</v>
       </c>
       <c r="D622" s="1" t="s">
-        <v>1176</v>
+        <v>329</v>
       </c>
       <c r="F622" s="1" t="s">
         <v>1366</v>
       </c>
     </row>
-    <row r="623" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="623" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A623" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B623,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/temperaturecorrection</v>
+        <v>class/attribute/temperature-f</v>
       </c>
       <c r="B623" s="1" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="C623" s="1" t="s">
-        <v>1463</v>
+        <v>1816</v>
       </c>
       <c r="D623" s="1" t="s">
-        <v>329</v>
+        <v>1176</v>
       </c>
       <c r="F623" s="1" t="s">
         <v>1366</v>
@@ -19011,7 +18981,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="644" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="644" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A644" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B644,",",""),"_","-")," ","-"))</f>
         <v>class/attribute/timesincecirculation</v>
@@ -19217,37 +19187,37 @@
     <row r="655" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A655" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B655,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/uncertainty-mgal</v>
+        <v>class/attribute/uncertaintydensity</v>
       </c>
       <c r="B655" s="1" t="s">
-        <v>1232</v>
+        <v>1234</v>
       </c>
       <c r="C655" s="1" t="s">
-        <v>1954</v>
+        <v>1234</v>
       </c>
       <c r="D655" s="1" t="s">
-        <v>1233</v>
+        <v>1235</v>
       </c>
       <c r="F655" s="1" t="s">
-        <v>1366</v>
+        <v>4</v>
       </c>
     </row>
     <row r="656" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A656" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B656,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/uncertaintydensity</v>
+        <v>class/attribute/uncertainty-mgal</v>
       </c>
       <c r="B656" s="1" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="C656" s="1" t="s">
-        <v>1234</v>
+        <v>1954</v>
       </c>
       <c r="D656" s="1" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="F656" s="1" t="s">
-        <v>4</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="657" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -19322,37 +19292,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="661" spans="1:8" ht="57" x14ac:dyDescent="0.2">
+    <row r="661" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A661" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B661,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/units-pressure</v>
+        <v>class/attribute/unitsofmeasure</v>
       </c>
       <c r="B661" s="1" t="s">
-        <v>1244</v>
+        <v>1247</v>
       </c>
       <c r="C661" s="1" t="s">
-        <v>1408</v>
+        <v>1418</v>
       </c>
       <c r="D661" s="1" t="s">
-        <v>1245</v>
+        <v>391</v>
       </c>
       <c r="F661" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="662" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="662" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A662" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B662,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/units-temperature</v>
+        <v>class/attribute/unitspermeability</v>
       </c>
       <c r="B662" s="1" t="s">
-        <v>1246</v>
+        <v>1248</v>
       </c>
       <c r="C662" s="1" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="D662" s="1" t="s">
-        <v>1174</v>
+        <v>1249</v>
       </c>
       <c r="F662" s="1" t="s">
         <v>4</v>
@@ -19361,34 +19331,34 @@
     <row r="663" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A663" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B663,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/unitsofmeasure</v>
+        <v>class/attribute/unitsporosity</v>
       </c>
       <c r="B663" s="1" t="s">
-        <v>1247</v>
+        <v>1250</v>
       </c>
       <c r="C663" s="1" t="s">
-        <v>1418</v>
+        <v>1411</v>
       </c>
       <c r="D663" s="1" t="s">
-        <v>391</v>
+        <v>1251</v>
       </c>
       <c r="F663" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="664" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A664" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B664,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/unitspermeability</v>
+        <v>class/attribute/units-pressure</v>
       </c>
       <c r="B664" s="1" t="s">
-        <v>1248</v>
+        <v>1244</v>
       </c>
       <c r="C664" s="1" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="D664" s="1" t="s">
-        <v>1249</v>
+        <v>1245</v>
       </c>
       <c r="F664" s="1" t="s">
         <v>4</v>
@@ -19397,55 +19367,55 @@
     <row r="665" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A665" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B665,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/unitsporosity</v>
+        <v>class/attribute/unitsstorage</v>
       </c>
       <c r="B665" s="1" t="s">
-        <v>1250</v>
+        <v>1252</v>
       </c>
       <c r="C665" s="1" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="D665" s="1" t="s">
-        <v>1251</v>
+        <v>1253</v>
       </c>
       <c r="F665" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="666" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="666" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A666" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B666,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/unitsstorage</v>
+        <v>class/attribute/unitstc</v>
       </c>
       <c r="B666" s="1" t="s">
-        <v>1252</v>
+        <v>1254</v>
       </c>
       <c r="C666" s="1" t="s">
-        <v>1412</v>
+        <v>1403</v>
       </c>
       <c r="D666" s="1" t="s">
-        <v>1253</v>
+        <v>1255</v>
       </c>
       <c r="F666" s="1" t="s">
-        <v>4</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="667" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A667" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B667,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/unitstc</v>
+        <v>class/attribute/units-temperature</v>
       </c>
       <c r="B667" s="1" t="s">
-        <v>1254</v>
+        <v>1246</v>
       </c>
       <c r="C667" s="1" t="s">
-        <v>1403</v>
+        <v>1409</v>
       </c>
       <c r="D667" s="1" t="s">
-        <v>1255</v>
+        <v>1174</v>
       </c>
       <c r="F667" s="1" t="s">
-        <v>1366</v>
+        <v>4</v>
       </c>
     </row>
     <row r="668" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -19529,40 +19499,40 @@
     <row r="672" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A672" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B672,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/utm-e</v>
+        <v>class/attribute/utmdatumzone</v>
       </c>
       <c r="B672" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C672" s="1" t="s">
-        <v>1955</v>
+        <v>1501</v>
       </c>
       <c r="D672" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E672" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E672" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F672" s="1" t="s">
-        <v>1366</v>
-      </c>
-      <c r="H672" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="G672" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="673" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A673" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B673,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/utm-n</v>
+        <v>class/attribute/utm-e</v>
       </c>
       <c r="B673" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C673" s="1" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="D673" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E673" s="1" t="s">
         <v>5</v>
@@ -19577,25 +19547,25 @@
     <row r="674" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A674" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B674,",",""),"_","-")," ","-"))</f>
-        <v>class/attribute/utmdatumzone</v>
+        <v>class/attribute/utm-n</v>
       </c>
       <c r="B674" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C674" s="1" t="s">
-        <v>1501</v>
+        <v>1956</v>
       </c>
       <c r="D674" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E674" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E674" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F674" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G674" s="1" t="s">
-        <v>3</v>
+        <v>1366</v>
+      </c>
+      <c r="H674" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="675" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -19619,7 +19589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="676" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="676" spans="1:8" ht="57" x14ac:dyDescent="0.2">
       <c r="A676" s="2" t="str">
         <f>"class/attribute/"&amp;LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B676,",",""),"_","-")," ","-"))</f>
         <v>class/attribute/ventelevation</v>
@@ -20276,22 +20246,22 @@
   </sheetData>
   <autoFilter ref="H1:H706"/>
   <sortState ref="A2:I709">
-    <sortCondition ref="B1"/>
+    <sortCondition ref="A1"/>
   </sortState>
   <conditionalFormatting sqref="C1:C2 C4:C704 C708:C1048576">
-    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C705">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C706">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C707">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>